<commit_message>
Masterfile issue fixed - UIn instead of U for inlet velocity
</commit_message>
<xml_diff>
--- a/variant_generator/Masterfile.xlsx
+++ b/variant_generator/Masterfile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t xml:space="preserve">PARAMETER</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">MANUAL</t>
   </si>
   <si>
-    <t xml:space="preserve">U</t>
+    <t xml:space="preserve">UIn</t>
   </si>
   <si>
     <t xml:space="preserve">geometric_progress</t>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">LIMITS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIn</t>
   </si>
   <si>
     <t xml:space="preserve">normal</t>
@@ -297,7 +294,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,7 +404,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -512,10 +509,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -530,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,7 +535,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10000</v>

</xml_diff>